<commit_message>
jadwal jam kerja dinamis
</commit_message>
<xml_diff>
--- a/public/import/master/jadwal.xlsx
+++ b/public/import/master/jadwal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23880" windowHeight="13820"/>
+    <workbookView windowHeight="15080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="4">
   <si>
-    <t>no_pegawai</t>
+    <t>no_ktp</t>
   </si>
   <si>
-    <t>Sh1</t>
+    <t>L</t>
   </si>
   <si>
-    <t>Sh2</t>
+    <t>SP8581</t>
+  </si>
+  <si>
+    <t>So7953</t>
   </si>
 </sst>
 </file>
@@ -30,10 +33,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -44,8 +47,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -59,25 +63,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,28 +78,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -129,6 +94,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -136,53 +125,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,181 +206,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,6 +418,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -430,26 +442,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,28 +492,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,133 +511,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -643,13 +643,16 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -681,39 +684,39 @@
     <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
-    <cellStyle name="Total" xfId="24" builtinId="25"/>
-    <cellStyle name="Output" xfId="25" builtinId="21"/>
-    <cellStyle name="Currency" xfId="26" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="Note" xfId="28" builtinId="10"/>
-    <cellStyle name="Input" xfId="29" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Good" xfId="32" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="Title" xfId="38" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
-    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
-    <cellStyle name="Link" xfId="43" builtinId="8"/>
-    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
-    <cellStyle name="Comma" xfId="45" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -980,19 +983,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="11.0625" customWidth="1"/>
     <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="32" width="5.59375" customWidth="1"/>
+    <col min="3" max="3" width="5.59375" customWidth="1"/>
+    <col min="4" max="4" width="7.75" customWidth="1"/>
+    <col min="5" max="32" width="5.59375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -1095,16 +1100,16 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
@@ -1113,10 +1118,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
@@ -1125,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>2</v>
@@ -1137,10 +1142,10 @@
         <v>1</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>2</v>
@@ -1149,46 +1154,46 @@
         <v>1</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>